<commit_message>
Nu med ELC-fuels trades
</commit_message>
<xml_diff>
--- a/TIMES-DE/Sets-TIMES_DE.xlsx
+++ b/TIMES-DE/Sets-TIMES_DE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\~g2v_TIMES_AZ\TIMES-AZ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0ee8d5d29f1698f/Desktop/GitHub/Bachelor_Git/TIMES-DE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D107CD2-1F72-4D70-85A0-AA251E07B107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{6D107CD2-1F72-4D70-85A0-AA251E07B107}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E80E2709-DEFA-4E8D-A03D-CE34DC1AE282}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{008F860A-1793-4F78-8899-BE3F7B7A437A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{008F860A-1793-4F78-8899-BE3F7B7A437A}"/>
   </bookViews>
   <sheets>
     <sheet name="SetsEditor- Comm" sheetId="4" r:id="rId1"/>
@@ -1044,7 +1044,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1346,17 +1346,17 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>102</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>109</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>107</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>106</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>105</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>104</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>111</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>112</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>113</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>116</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>138</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>191</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>221</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>224</v>
       </c>
@@ -1711,22 +1711,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C483E65-AD60-4207-9D9B-29377F595575}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="24.7265625" customWidth="1"/>
+    <col min="11" max="11" width="19.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -1761,7 +1763,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -1790,7 +1792,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1819,7 +1821,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -1848,7 +1850,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>61</v>
       </c>
@@ -1877,7 +1879,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -1906,7 +1908,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -1935,7 +1937,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>61</v>
       </c>
@@ -1958,7 +1960,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>61</v>
       </c>
@@ -1987,7 +1989,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>61</v>
       </c>
@@ -2016,7 +2018,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -2045,7 +2047,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -2074,7 +2076,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -2103,7 +2105,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -2129,7 +2131,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -2155,7 +2157,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -2181,7 +2183,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -2207,7 +2209,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -2233,7 +2235,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>61</v>
       </c>
@@ -2259,7 +2261,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>61</v>
       </c>
@@ -2282,7 +2284,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -2308,7 +2310,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -2331,7 +2333,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -2354,7 +2356,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -2377,7 +2379,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2400,7 +2402,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -2423,7 +2425,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -2446,7 +2448,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -2469,7 +2471,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -2492,7 +2494,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>61</v>
       </c>
@@ -2515,7 +2517,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -2538,7 +2540,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>61</v>
       </c>
@@ -2561,7 +2563,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -2584,7 +2586,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>61</v>
       </c>
@@ -2607,7 +2609,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -2630,7 +2632,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>61</v>
       </c>
@@ -2656,7 +2658,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>61</v>
       </c>
@@ -2679,7 +2681,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>61</v>
       </c>
@@ -2702,7 +2704,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>61</v>
       </c>
@@ -2725,7 +2727,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>61</v>
       </c>
@@ -2748,7 +2750,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>61</v>
       </c>
@@ -2774,7 +2776,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>61</v>
       </c>
@@ -2800,7 +2802,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>61</v>
       </c>
@@ -2826,7 +2828,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>61</v>
       </c>
@@ -2852,7 +2854,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>61</v>
       </c>
@@ -2878,7 +2880,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -2904,7 +2906,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>61</v>
       </c>
@@ -2930,7 +2932,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>61</v>
       </c>
@@ -2956,7 +2958,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -2982,7 +2984,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>61</v>
       </c>
@@ -3008,7 +3010,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -3037,7 +3039,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -3066,7 +3068,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>61</v>
       </c>
@@ -3092,7 +3094,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>61</v>
       </c>
@@ -3115,7 +3117,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>61</v>
       </c>
@@ -3138,7 +3140,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -3164,7 +3166,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>61</v>
       </c>
@@ -3187,7 +3189,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -3216,7 +3218,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -3245,7 +3247,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -3274,7 +3276,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -3303,7 +3305,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -3332,7 +3334,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -3361,7 +3363,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>61</v>
       </c>
@@ -3393,7 +3395,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>61</v>
       </c>
@@ -3422,7 +3424,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>61</v>
       </c>
@@ -3448,7 +3450,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>61</v>
       </c>
@@ -3487,23 +3489,23 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -3529,7 +3531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
         <v>23</v>
       </c>
@@ -3559,18 +3561,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" customWidth="1"/>
+    <col min="7" max="7" width="23.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3602,7 +3604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>11</v>
       </c>
@@ -3619,7 +3621,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>14</v>
       </c>
@@ -3636,7 +3638,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -3656,7 +3658,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>25</v>
       </c>
@@ -3679,6 +3681,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100391E4ED4D6B5344984C5B5CBC1A28781" ma:contentTypeVersion="13" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="a8662b4a95e495bc977359cc4b8d0a5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6218e30f-ac19-4e1a-9d42-0577826d9887" xmlns:ns3="9bef2f80-48e4-49d2-aa34-66e9d7fcf80f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b72a6a49e693c9bb3f1300811353490c" ns2:_="" ns3:_="">
     <xsd:import namespace="6218e30f-ac19-4e1a-9d42-0577826d9887"/>
@@ -3901,29 +3918,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0515B61-51E1-43C6-B93C-47051DC1E891}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D21B4D4-0580-4DC5-8C48-67FE9BC1B49A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1082D17A-6642-4FF2-A329-E0977A24CD02}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1082D17A-6642-4FF2-A329-E0977A24CD02}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D21B4D4-0580-4DC5-8C48-67FE9BC1B49A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0515B61-51E1-43C6-B93C-47051DC1E891}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6218e30f-ac19-4e1a-9d42-0577826d9887"/>
+    <ds:schemaRef ds:uri="9bef2f80-48e4-49d2-aa34-66e9d7fcf80f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>